<commit_message>
Deploy Fatigue Detection App to Streamlit Cloud
</commit_message>
<xml_diff>
--- a/metrics.xlsx
+++ b/metrics.xlsx
@@ -506,19 +506,19 @@
         <v>9</v>
       </c>
       <c r="B5">
-        <v>0.8798418972332016</v>
+        <v>0.88300395256917</v>
       </c>
       <c r="C5">
-        <v>0.8703703703703703</v>
+        <v>0.8740053050397878</v>
       </c>
       <c r="D5">
-        <v>0.9241573033707865</v>
+        <v>0.925561797752809</v>
       </c>
       <c r="E5">
-        <v>0.896457765667575</v>
+        <v>0.8990450204638472</v>
       </c>
       <c r="F5">
-        <v>0.9545279070239958</v>
+        <v>0.9545990206635919</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -526,19 +526,19 @@
         <v>10</v>
       </c>
       <c r="B6">
-        <v>0.916205533596838</v>
+        <v>0.9146245059288538</v>
       </c>
       <c r="C6">
-        <v>0.9116847826086957</v>
+        <v>0.9081081081081082</v>
       </c>
       <c r="D6">
-        <v>0.9424157303370787</v>
+        <v>0.9438202247191011</v>
       </c>
       <c r="E6">
-        <v>0.9267955801104972</v>
+        <v>0.9256198347107438</v>
       </c>
       <c r="F6">
-        <v>0.9694363736107442</v>
+        <v>0.9692255724647987</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -546,19 +546,19 @@
         <v>11</v>
       </c>
       <c r="B7">
-        <v>0.9217391304347826</v>
+        <v>0.9225296442687747</v>
       </c>
       <c r="C7">
-        <v>0.9359886201991465</v>
+        <v>0.9299719887955182</v>
       </c>
       <c r="D7">
-        <v>0.9241573033707865</v>
+        <v>0.9325842696629213</v>
       </c>
       <c r="E7">
-        <v>0.9300353356890459</v>
+        <v>0.9312762973352033</v>
       </c>
       <c r="G7">
-        <v>0.5600000000000002</v>
+        <v>0.5400000000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>